<commit_message>
add discount categories and styles.
</commit_message>
<xml_diff>
--- a/discount listing.xlsx
+++ b/discount listing.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="83">
   <si>
     <t>Initial price</t>
   </si>
@@ -221,9 +221,6 @@
     <t>SHORT &amp; SHIRT</t>
   </si>
   <si>
-    <t>FLORAL DRESS</t>
-  </si>
-  <si>
     <t>BODY SUIT</t>
   </si>
   <si>
@@ -261,13 +258,28 @@
   </si>
   <si>
     <t>SPORTS BRA</t>
+  </si>
+  <si>
+    <t>BABY CLOTHING SET</t>
+  </si>
+  <si>
+    <t>Home &amp; Garden</t>
+  </si>
+  <si>
+    <t>BULB CHANDELIER</t>
+  </si>
+  <si>
+    <t>BATHROOM FIXTURE</t>
+  </si>
+  <si>
+    <t>GARDEN FOUNTAIN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,13 +337,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -348,7 +380,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -364,6 +396,10 @@
     </xf>
     <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -646,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69:G69"/>
+      <selection activeCell="G76" sqref="G76:G80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,7 +737,7 @@
       <c r="F3" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="16" t="s">
         <v>51</v>
       </c>
     </row>
@@ -726,7 +762,7 @@
       <c r="F4" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="16" t="s">
         <v>51</v>
       </c>
     </row>
@@ -751,7 +787,7 @@
       <c r="F5" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="16" t="s">
         <v>50</v>
       </c>
     </row>
@@ -776,7 +812,7 @@
       <c r="F6" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="16" t="s">
         <v>49</v>
       </c>
     </row>
@@ -801,7 +837,7 @@
       <c r="F7" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="16" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1009,7 +1045,7 @@
       <c r="F17" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="16" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1034,7 +1070,7 @@
       <c r="F18" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="16" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1059,7 +1095,7 @@
       <c r="F19" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="16" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1084,7 +1120,7 @@
       <c r="F20" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="16" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1314,7 +1350,7 @@
       <c r="F32" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" s="16" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1339,7 +1375,7 @@
       <c r="F33" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33" s="16" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1364,7 +1400,7 @@
       <c r="F34" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34" s="16" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1389,7 +1425,7 @@
       <c r="F35" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G35" s="16" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1414,7 +1450,7 @@
       <c r="F36" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="16" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1613,13 +1649,13 @@
         <v>1500</v>
       </c>
       <c r="E47" s="5">
-        <f t="shared" ref="E47:E62" si="7">D47/B47</f>
+        <f t="shared" ref="E47:E58" si="7">D47/B47</f>
         <v>0.25</v>
       </c>
       <c r="F47" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G47" s="16" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1634,7 +1670,7 @@
         <v>2300.9899999999998</v>
       </c>
       <c r="D48">
-        <f t="shared" ref="D48:D62" si="8">B48-C48</f>
+        <f t="shared" ref="D48:D58" si="8">B48-C48</f>
         <v>199.01000000000022</v>
       </c>
       <c r="E48" s="5">
@@ -1644,7 +1680,7 @@
       <c r="F48" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G48" s="16" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1669,7 +1705,7 @@
       <c r="F49" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G49" s="16" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1694,7 +1730,7 @@
       <c r="F50" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G50" s="16" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1828,14 +1864,14 @@
         <v>64</v>
       </c>
       <c r="B56" s="3">
-        <v>31500</v>
+        <v>3150</v>
       </c>
       <c r="C56" s="4">
-        <v>25000</v>
+        <v>2500</v>
       </c>
       <c r="D56">
         <f t="shared" si="8"/>
-        <v>6500</v>
+        <v>650</v>
       </c>
       <c r="E56" s="5">
         <f t="shared" si="7"/>
@@ -1850,32 +1886,32 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>65</v>
-      </c>
-      <c r="B57" s="9">
-        <v>2500</v>
-      </c>
-      <c r="C57" s="11">
-        <v>1500</v>
+        <v>78</v>
+      </c>
+      <c r="B57" s="3">
+        <v>4000</v>
+      </c>
+      <c r="C57" s="4">
+        <v>2000</v>
       </c>
       <c r="D57">
         <f t="shared" si="8"/>
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="E57" s="5">
         <f t="shared" si="7"/>
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G57" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B58" s="9">
         <v>2000</v>
@@ -1909,7 +1945,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B61" s="9">
         <v>30000</v>
@@ -1928,13 +1964,13 @@
       <c r="F61" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G61" s="16" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B62" s="6">
         <v>16000</v>
@@ -1953,13 +1989,13 @@
       <c r="F62" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G62" t="s">
+      <c r="G62" s="16" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B63" s="6">
         <v>9000</v>
@@ -1978,13 +2014,13 @@
       <c r="F63" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G63" s="16" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B64" s="6">
         <v>39999</v>
@@ -2003,13 +2039,13 @@
       <c r="F64" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="G64" t="s">
+      <c r="G64" s="16" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B65" s="9">
         <v>1500</v>
@@ -2028,13 +2064,13 @@
       <c r="F65" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="G65" t="s">
+      <c r="G65" s="16" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B66" s="9">
         <v>10000</v>
@@ -2059,7 +2095,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B67" s="9">
         <v>1000</v>
@@ -2084,7 +2120,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B68" s="6">
         <v>3500</v>
@@ -2109,7 +2145,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B69" s="9">
         <v>5000</v>
@@ -2134,7 +2170,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B70" s="6">
         <v>3000</v>
@@ -2159,7 +2195,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B71" s="9">
         <v>3500</v>
@@ -2184,7 +2220,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B72" s="9">
         <v>2000</v>
@@ -2207,53 +2243,366 @@
         <v>50</v>
       </c>
     </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>80</v>
+      </c>
+      <c r="B76" s="13">
+        <v>20000</v>
+      </c>
+      <c r="C76" s="14">
+        <v>16900</v>
+      </c>
+      <c r="D76">
+        <f>B76-C76</f>
+        <v>3100</v>
+      </c>
+      <c r="E76" s="5">
+        <f t="shared" ref="E76:E87" si="13">D76/B76</f>
+        <v>0.155</v>
+      </c>
+      <c r="F76" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G76" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>80</v>
+      </c>
+      <c r="B77" s="13">
+        <v>25000</v>
+      </c>
+      <c r="C77" s="15">
+        <v>23000.99</v>
+      </c>
+      <c r="D77">
+        <f t="shared" ref="D77:D87" si="14">B77-C77</f>
+        <v>1999.0099999999984</v>
+      </c>
+      <c r="E77" s="5">
+        <f t="shared" si="13"/>
+        <v>7.9960399999999932E-2</v>
+      </c>
+      <c r="F77" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G77" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>80</v>
+      </c>
+      <c r="B78" s="13">
+        <v>23900</v>
+      </c>
+      <c r="C78" s="15">
+        <v>14900</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="14"/>
+        <v>9000</v>
+      </c>
+      <c r="E78" s="5">
+        <f t="shared" si="13"/>
+        <v>0.37656903765690375</v>
+      </c>
+      <c r="F78" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G78" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>80</v>
+      </c>
+      <c r="B79" s="13">
+        <v>31500</v>
+      </c>
+      <c r="C79" s="15">
+        <v>25000</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="14"/>
+        <v>6500</v>
+      </c>
+      <c r="E79" s="5">
+        <f t="shared" si="13"/>
+        <v>0.20634920634920634</v>
+      </c>
+      <c r="F79" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G79" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>81</v>
+      </c>
+      <c r="B80" s="13">
+        <v>7000</v>
+      </c>
+      <c r="C80" s="15">
+        <v>5000</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="14"/>
+        <v>2000</v>
+      </c>
+      <c r="E80" s="5">
+        <f t="shared" si="13"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="F80" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G80" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>81</v>
+      </c>
+      <c r="B81" s="9">
+        <v>3500</v>
+      </c>
+      <c r="C81" s="15">
+        <v>2500</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="14"/>
+        <v>1000</v>
+      </c>
+      <c r="E81" s="5">
+        <f t="shared" si="13"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="F81" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G81" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>81</v>
+      </c>
+      <c r="B82" s="9">
+        <v>5000</v>
+      </c>
+      <c r="C82" s="4">
+        <v>4000</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="14"/>
+        <v>1000</v>
+      </c>
+      <c r="E82" s="5">
+        <f t="shared" si="13"/>
+        <v>0.2</v>
+      </c>
+      <c r="F82" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G82" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>81</v>
+      </c>
+      <c r="B83" s="6">
+        <v>5000</v>
+      </c>
+      <c r="C83" s="8">
+        <v>3000</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="14"/>
+        <v>2000</v>
+      </c>
+      <c r="E83" s="5">
+        <f t="shared" si="13"/>
+        <v>0.4</v>
+      </c>
+      <c r="F83" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G83" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>82</v>
+      </c>
+      <c r="B84" s="9">
+        <v>36900</v>
+      </c>
+      <c r="C84" s="8">
+        <v>34900</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="14"/>
+        <v>2000</v>
+      </c>
+      <c r="E84" s="5">
+        <f t="shared" si="13"/>
+        <v>5.4200542005420058E-2</v>
+      </c>
+      <c r="F84" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G84" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>82</v>
+      </c>
+      <c r="B85" s="6">
+        <v>31500</v>
+      </c>
+      <c r="C85" s="8">
+        <v>25000</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="14"/>
+        <v>6500</v>
+      </c>
+      <c r="E85" s="5">
+        <f t="shared" si="13"/>
+        <v>0.20634920634920634</v>
+      </c>
+      <c r="F85" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G85" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>82</v>
+      </c>
+      <c r="B86" s="9">
+        <v>45000</v>
+      </c>
+      <c r="C86" s="11">
+        <v>41800</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="14"/>
+        <v>3200</v>
+      </c>
+      <c r="E86" s="5">
+        <f t="shared" si="13"/>
+        <v>7.1111111111111111E-2</v>
+      </c>
+      <c r="F86" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G86" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>82</v>
+      </c>
+      <c r="B87" s="9">
+        <v>35000</v>
+      </c>
+      <c r="C87" s="8">
+        <v>33000</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="14"/>
+        <v>2000</v>
+      </c>
+      <c r="E87" s="5">
+        <f t="shared" si="13"/>
+        <v>5.7142857142857141E-2</v>
+      </c>
+      <c r="F87" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G87" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F6"/>
-    <hyperlink ref="F8"/>
-    <hyperlink ref="F12"/>
-    <hyperlink ref="F17"/>
-    <hyperlink ref="F21"/>
-    <hyperlink ref="F28"/>
-    <hyperlink ref="F25"/>
-    <hyperlink ref="F5"/>
-    <hyperlink ref="F18"/>
-    <hyperlink ref="F20"/>
-    <hyperlink ref="F22:F24"/>
-    <hyperlink ref="F26"/>
-    <hyperlink ref="F33"/>
-    <hyperlink ref="F35"/>
-    <hyperlink ref="F37"/>
-    <hyperlink ref="F38:F39"/>
-    <hyperlink ref="F41"/>
-    <hyperlink ref="F32"/>
-    <hyperlink ref="F40"/>
-    <hyperlink ref="F43"/>
-    <hyperlink ref="F36"/>
-    <hyperlink ref="F42"/>
-    <hyperlink ref="F27"/>
-    <hyperlink ref="F67"/>
-    <hyperlink ref="F49"/>
-    <hyperlink ref="F52"/>
-    <hyperlink ref="F57"/>
-    <hyperlink ref="F61"/>
-    <hyperlink ref="F64"/>
-    <hyperlink ref="F65"/>
-    <hyperlink ref="F66"/>
-    <hyperlink ref="F68"/>
-    <hyperlink ref="F50"/>
-    <hyperlink ref="F51"/>
-    <hyperlink ref="F56"/>
-    <hyperlink ref="F63"/>
-    <hyperlink ref="F62"/>
-    <hyperlink ref="F58"/>
-    <hyperlink ref="F55"/>
-    <hyperlink ref="F54"/>
-    <hyperlink ref="F47"/>
-    <hyperlink ref="F72"/>
-    <hyperlink ref="F71"/>
-    <hyperlink ref="F70"/>
-    <hyperlink ref="F69"/>
+    <hyperlink ref="F6" display="Over 10% Discounts"/>
+    <hyperlink ref="F8" display="Over 10% Discounts"/>
+    <hyperlink ref="F12" display="Over 10% Discounts"/>
+    <hyperlink ref="F17" display="Over 10% Discounts"/>
+    <hyperlink ref="F21" display="Over 10% Discounts"/>
+    <hyperlink ref="F28" display="Over 10% Discounts"/>
+    <hyperlink ref="F25" display="Over 10% Discounts"/>
+    <hyperlink ref="F5" display="Over 25% Discounts"/>
+    <hyperlink ref="F18" display="Over 25% Discounts"/>
+    <hyperlink ref="F20" display="Over 25% Discounts"/>
+    <hyperlink ref="F22:F24" display="Over 25% Discounts"/>
+    <hyperlink ref="F26" display="Over 25% Discounts"/>
+    <hyperlink ref="F33" display="Over 25% Discounts"/>
+    <hyperlink ref="F35" display="Over 25% Discounts"/>
+    <hyperlink ref="F37" display="Over 25% Discounts"/>
+    <hyperlink ref="F38:F39" display="Over 25% Discounts"/>
+    <hyperlink ref="F41" display="Over 25% Discounts"/>
+    <hyperlink ref="F32" display="Over 10% Discounts"/>
+    <hyperlink ref="F40" display="Over 10% Discounts"/>
+    <hyperlink ref="F43" display="Over 10% Discounts"/>
+    <hyperlink ref="F36" display="Over 10% Discounts"/>
+    <hyperlink ref="F42" display="Over 40% Discounts"/>
+    <hyperlink ref="F27" display="Over 40% Discounts"/>
+    <hyperlink ref="F67" display="Over 25% Discounts"/>
+    <hyperlink ref="F49" display="Over 40% Discounts"/>
+    <hyperlink ref="F52" display="Over 40% Discounts"/>
+    <hyperlink ref="F57" display="Over 40% Discounts"/>
+    <hyperlink ref="F61" display="Over 50% Discounts"/>
+    <hyperlink ref="F64" display="Over 50% Discounts"/>
+    <hyperlink ref="F65" display="Over 50% Discounts"/>
+    <hyperlink ref="F66" display="Over 50% Discounts"/>
+    <hyperlink ref="F68" display="Over 50% Discounts"/>
+    <hyperlink ref="F50" display="Over 10% Discounts"/>
+    <hyperlink ref="F51" display="Over 10% Discounts"/>
+    <hyperlink ref="F56" display="Over 10% Discounts"/>
+    <hyperlink ref="F63" display="Over 10% Discounts"/>
+    <hyperlink ref="F62" display="Over 25% Discounts"/>
+    <hyperlink ref="F58" display="Over 25% Discounts"/>
+    <hyperlink ref="F55" display="Over 25% Discounts"/>
+    <hyperlink ref="F54" display="Over 25% Discounts"/>
+    <hyperlink ref="F47" display="Over 25% Discounts"/>
+    <hyperlink ref="F72" display="Over 25% Discounts"/>
+    <hyperlink ref="F71" display="Over 25% Discounts"/>
+    <hyperlink ref="F70" display="Over 50% Discounts"/>
+    <hyperlink ref="F69" display="Over 25% Discounts"/>
+    <hyperlink ref="F80" display="Over 25% Discounts"/>
+    <hyperlink ref="F81" display="Over 25% Discounts"/>
+    <hyperlink ref="F78" display="Over 25% Discounts"/>
+    <hyperlink ref="F76" display="Over 10% Discounts"/>
+    <hyperlink ref="F79" display="Over 10% Discounts"/>
+    <hyperlink ref="F82" display="Over 10% Discounts"/>
+    <hyperlink ref="F83" display="Over 40% Discounts"/>
+    <hyperlink ref="F85" display="Over 10% Discounts"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>